<commit_message>
adding items to BOM
</commit_message>
<xml_diff>
--- a/PCB/BOM_Spreadsheet.xlsx
+++ b/PCB/BOM_Spreadsheet.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="223">
   <si>
     <t>Qty</t>
   </si>
@@ -610,9 +610,6 @@
     <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM155R60J102KA01D/490-6285-1-ND/3845482</t>
   </si>
   <si>
-    <t>Spare 9 ordered (cheaper than just 3)</t>
-  </si>
-  <si>
     <t>311-10.0HRCT-ND</t>
   </si>
   <si>
@@ -622,16 +619,109 @@
     <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-0710RL/311-10.0HRCT-ND/729826</t>
   </si>
   <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>490-3194-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM033R71A103KA01D/490-3194-1-ND/702735</t>
-  </si>
-  <si>
-    <t>GRM033R71A103KA01D</t>
+    <t>399-7835-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C102K4RACTU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0603C102K4RACTU/399-7835-1-ND/3471558</t>
+  </si>
+  <si>
+    <t>Spare 6 ordered</t>
+  </si>
+  <si>
+    <t>P10KBYCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-PA3F1002V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PA3F1002V/P10KBYCT-ND/5036115</t>
+  </si>
+  <si>
+    <t>490-7198-1-ND</t>
+  </si>
+  <si>
+    <t>GRM188C81C106MA73D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM188C81C106MA73D/490-7198-1-ND/3900421</t>
+  </si>
+  <si>
+    <t>Spare 4 ordered</t>
+  </si>
+  <si>
+    <t>10000pF</t>
+  </si>
+  <si>
+    <t>399-7841-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C103K4RACTU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0603C103K4RACTU/399-7841-1-ND/3471564</t>
+  </si>
+  <si>
+    <t>493-11461-1-ND</t>
+  </si>
+  <si>
+    <t>UPM1E151MPD1TD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/nichicon/UPM1E151MPD1TD/493-11461-1-ND/4319571</t>
+  </si>
+  <si>
+    <t>490-1198-1-ND</t>
+  </si>
+  <si>
+    <t>CSTCE16M0V53-R0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/CSTCE16M0V53-R0/490-1198-1-ND/584635</t>
+  </si>
+  <si>
+    <t>399-11141-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C180J4GACTU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0603C180J4GACTU/399-11141-1-ND/4357831</t>
+  </si>
+  <si>
+    <t>311-1.00MHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-071ML</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-071ML/311-1.00MHRCT-ND/729791</t>
+  </si>
+  <si>
+    <t>1276-1019-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B105KO8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL10B105KO8NNNC/1276-1019-1-ND/3889105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spare 9 ordered </t>
+  </si>
+  <si>
+    <t>Spare 9 ordered</t>
+  </si>
+  <si>
+    <t>490-5255-1-ND</t>
+  </si>
+  <si>
+    <t>BLM18KG221SN1D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/BLM18KG221SN1D/490-5255-1-ND/1982778</t>
   </si>
 </sst>
 </file>
@@ -691,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -703,6 +793,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1024,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,6 +1137,7 @@
     <col min="13" max="13" width="18.5703125" customWidth="1"/>
     <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="19" max="19" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -1347,10 +1439,10 @@
         <v>0.10999999999999999</v>
       </c>
       <c r="S7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1370,16 +1462,16 @@
         <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N8" t="s">
         <v>161</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q8">
         <v>1.4E-2</v>
@@ -1389,7 +1481,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S8" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1397,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -1411,32 +1503,31 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>192</v>
+      <c r="G9" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="N9" t="s">
         <v>161</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="P9" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="Q9">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="R9">
-        <f t="shared" si="0"/>
-        <v>0.21000000000000002</v>
+        <v>0.19</v>
       </c>
       <c r="S9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -1453,17 +1544,32 @@
       <c r="F10" t="s">
         <v>29</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="N10" t="s">
         <v>161</v>
       </c>
+      <c r="O10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P10" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q10">
+        <v>2.7E-2</v>
+      </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0.27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -1480,17 +1586,32 @@
       <c r="F11" t="s">
         <v>37</v>
       </c>
+      <c r="G11" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="N11" t="s">
         <v>161</v>
       </c>
+      <c r="O11" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="P11" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q11">
+        <v>0.13400000000000001</v>
+      </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="S11" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
@@ -1507,17 +1628,32 @@
       <c r="F12" t="s">
         <v>29</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="N12" t="s">
         <v>161</v>
       </c>
+      <c r="O12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q12">
+        <v>0.254</v>
+      </c>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.54</v>
+      </c>
+      <c r="S12" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
@@ -1534,17 +1670,32 @@
       <c r="F13" t="s">
         <v>49</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="N13" t="s">
         <v>161</v>
       </c>
+      <c r="O13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P13" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q13">
+        <v>0.22</v>
+      </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S13" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
@@ -1561,6 +1712,9 @@
       <c r="F14" t="s">
         <v>54</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="J14" t="s">
         <v>55</v>
       </c>
@@ -1570,14 +1724,26 @@
       <c r="N14" t="s">
         <v>161</v>
       </c>
+      <c r="O14" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P14" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q14">
+        <v>0.5</v>
+      </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="S14" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
@@ -1594,17 +1760,32 @@
       <c r="F15" t="s">
         <v>29</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="N15" t="s">
         <v>161</v>
       </c>
+      <c r="O15" t="s">
+        <v>209</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q15">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="S15" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>58</v>
@@ -1621,17 +1802,32 @@
       <c r="F16" t="s">
         <v>37</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="N16" t="s">
         <v>161</v>
       </c>
+      <c r="O16" t="s">
+        <v>212</v>
+      </c>
+      <c r="P16" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q16">
+        <v>1.4E-2</v>
+      </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
@@ -1648,15 +1844,30 @@
       <c r="F17" t="s">
         <v>29</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="N17" t="s">
         <v>161</v>
       </c>
+      <c r="O17" t="s">
+        <v>215</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q17">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="R17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.42999999999999994</v>
+      </c>
+      <c r="S17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1672,20 +1883,24 @@
       <c r="E18" t="s">
         <v>64</v>
       </c>
+      <c r="G18" s="1"/>
       <c r="H18">
         <v>2</v>
       </c>
       <c r="I18" t="s">
         <v>65</v>
       </c>
+      <c r="N18" t="s">
+        <v>161</v>
+      </c>
       <c r="R18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
@@ -1702,18 +1917,36 @@
       <c r="F19" t="s">
         <v>69</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="J19" t="s">
         <v>70</v>
       </c>
       <c r="M19" t="s">
         <v>71</v>
       </c>
+      <c r="N19" t="s">
+        <v>161</v>
+      </c>
+      <c r="O19" t="s">
+        <v>220</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q19">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="R19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="S19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1732,12 +1965,15 @@
       <c r="F20" t="s">
         <v>29</v>
       </c>
+      <c r="N20" t="s">
+        <v>161</v>
+      </c>
       <c r="R20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1767,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1791,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1815,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1839,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1863,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1887,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1908,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1932,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1956,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1977,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2007,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2375,8 +2611,12 @@
     <hyperlink ref="P4" r:id="rId1"/>
     <hyperlink ref="P5" r:id="rId2"/>
     <hyperlink ref="P6" r:id="rId3"/>
+    <hyperlink ref="P12" r:id="rId4"/>
+    <hyperlink ref="P15" r:id="rId5"/>
+    <hyperlink ref="P17" r:id="rId6"/>
+    <hyperlink ref="P19" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further added to BOM
</commit_message>
<xml_diff>
--- a/PCB/BOM_Spreadsheet.xlsx
+++ b/PCB/BOM_Spreadsheet.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="279">
   <si>
     <t>Qty</t>
   </si>
@@ -722,6 +722,174 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/BLM18KG221SN1D/490-5255-1-ND/1982778</t>
+  </si>
+  <si>
+    <t>C1608X5R1A226M080AC</t>
+  </si>
+  <si>
+    <t>445-9077-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1A226M080AC/445-9077-1-ND/3661620</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/abracon-llc/ABM3B-24.000MHZ-B4Y-T/535-13448-1-ND/5980124</t>
+  </si>
+  <si>
+    <t>535-13448-1-ND</t>
+  </si>
+  <si>
+    <t>ABM3B-24.000MHZ-B4Y-T</t>
+  </si>
+  <si>
+    <t>311-25.5KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-9.53KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-90.9KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0725K5L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-0725K5L/311-25.5KHRCT-ND/730035</t>
+  </si>
+  <si>
+    <t>spare 8 ordered</t>
+  </si>
+  <si>
+    <t>311-4.7KGRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>spare 1 ordered</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603JR-074K7L/311-4.7KGRCT-ND/729732</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/CC0603KRX5R7BB475/311-1785-1-ND/5195687</t>
+  </si>
+  <si>
+    <t>311-1785-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603KRX5R7BB475</t>
+  </si>
+  <si>
+    <t>541-3301-1-ND</t>
+  </si>
+  <si>
+    <t>TNPU0603500RAZEN00</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/vishay-dale/TNPU0603500RAZEN00/541-3301-1-ND/6615958</t>
+  </si>
+  <si>
+    <t>RMCF0603JT680RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT680R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603JT680R/RMCF0603JT680RCT-ND/1943169</t>
+  </si>
+  <si>
+    <t>Spare 1 ordered</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/fairchild-on-semiconductor/74VHC157MX/74VHC157MXCT-ND/4744147</t>
+  </si>
+  <si>
+    <t>74VHC157MXCT-ND</t>
+  </si>
+  <si>
+    <t>74VHC157MX</t>
+  </si>
+  <si>
+    <t>RC0603FR-079K53L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-079K53L/311-9.53KHRCT-ND/730368</t>
+  </si>
+  <si>
+    <t>spare 9 ordered</t>
+  </si>
+  <si>
+    <t>RC0603FR-0790K9L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0603FR-0790K9L/311-90.9KHRCT-ND/730371</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AURCT-ND</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AUR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-AUR/ATMEGA328P-AURCT-ND/3789455</t>
+  </si>
+  <si>
+    <t>ATTINY441-SSU-ND</t>
+  </si>
+  <si>
+    <t>ATTINY441-SSU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATTINY441-SSU/ATTINY441-SSU-ND/4437432</t>
+  </si>
+  <si>
+    <t>AZ1117CR-3.3TRG1</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/diodes-incorporated/AZ1117CR-3.3TRG1/AZ1117CR-3.3TRG1DICT-ND/5267011</t>
+  </si>
+  <si>
+    <t>S9197-ND</t>
+  </si>
+  <si>
+    <t>SFH11-PBPC-D10-ST-BK</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/SFH11-PBPC-D10-ST-BK/S9197-ND/1990090</t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>LM340SX-5.0/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>LM340SX-5.0/NOPB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/LM340SX-5.0-NOPB/LM340SX-5.0-NOPBCT-ND/6174310</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/c-k/RS-187R05A2-DS-MT-RT/CKN10361CT-ND/2747199</t>
+  </si>
+  <si>
+    <t>CKN10361CT-ND</t>
+  </si>
+  <si>
+    <t>RS-187R05A2-DS MT RT</t>
+  </si>
+  <si>
+    <t>1568-1391-ND</t>
+  </si>
+  <si>
+    <t>COM-13910</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sparkfun-electronics/COM-13910/1568-1391-ND/6023501</t>
   </si>
 </sst>
 </file>
@@ -751,12 +919,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -781,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -794,6 +968,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1115,18 +1290,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" hidden="1" customWidth="1"/>
@@ -1890,9 +2065,6 @@
       <c r="I18" t="s">
         <v>65</v>
       </c>
-      <c r="N18" t="s">
-        <v>161</v>
-      </c>
       <c r="R18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1948,7 +2120,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
@@ -1965,17 +2137,32 @@
       <c r="F20" t="s">
         <v>29</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="N20" t="s">
         <v>161</v>
       </c>
+      <c r="O20" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="P20" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q20">
+        <v>0.49</v>
+      </c>
       <c r="R20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.47</v>
+      </c>
+      <c r="S20" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>74</v>
@@ -1989,6 +2176,9 @@
       <c r="E21" t="s">
         <v>77</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="I21" t="s">
         <v>78</v>
       </c>
@@ -1998,9 +2188,24 @@
       <c r="L21" t="s">
         <v>74</v>
       </c>
+      <c r="N21" t="s">
+        <v>161</v>
+      </c>
+      <c r="O21" t="s">
+        <v>227</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q21">
+        <v>0.73</v>
+      </c>
       <c r="R21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.19</v>
+      </c>
+      <c r="S21" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -2022,9 +2227,27 @@
       <c r="F22" t="s">
         <v>37</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="N22" t="s">
+        <v>161</v>
+      </c>
+      <c r="O22" t="s">
+        <v>229</v>
+      </c>
+      <c r="P22" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q22">
+        <v>1.4E-2</v>
+      </c>
       <c r="R22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="S22" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2046,14 +2269,32 @@
       <c r="F23" t="s">
         <v>37</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N23" t="s">
+        <v>161</v>
+      </c>
+      <c r="O23" t="s">
+        <v>235</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q23">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="R23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="S23" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
@@ -2070,14 +2311,32 @@
       <c r="F24" t="s">
         <v>29</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" t="s">
+        <v>161</v>
+      </c>
+      <c r="O24" t="s">
+        <v>240</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q24">
+        <v>0.25</v>
+      </c>
       <c r="R24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
+      </c>
+      <c r="S24" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <v>500</v>
@@ -2094,14 +2353,32 @@
       <c r="F25" t="s">
         <v>37</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="N25" t="s">
+        <v>161</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P25" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q25">
+        <v>3.17</v>
+      </c>
       <c r="R25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.34</v>
+      </c>
+      <c r="S25" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>680</v>
@@ -2118,14 +2395,32 @@
       <c r="F26" t="s">
         <v>37</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="N26" t="s">
+        <v>161</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="P26" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q26">
+        <v>1.2999999999999999E-2</v>
+      </c>
       <c r="R26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0.13</v>
+      </c>
+      <c r="S26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>88</v>
@@ -2139,14 +2434,32 @@
       <c r="E27" t="s">
         <v>90</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="N27" t="s">
+        <v>161</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q27">
+        <v>0.59</v>
+      </c>
       <c r="R27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.77</v>
+      </c>
+      <c r="S27" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
         <v>91</v>
@@ -2163,9 +2476,27 @@
       <c r="F28" t="s">
         <v>37</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N28" t="s">
+        <v>161</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q28">
+        <v>1.4E-2</v>
+      </c>
       <c r="R28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S28" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2187,35 +2518,68 @@
       <c r="F29" t="s">
         <v>37</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="N29" t="s">
+        <v>161</v>
+      </c>
+      <c r="O29" t="s">
+        <v>231</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q29">
+        <v>1.4E-2</v>
+      </c>
       <c r="R29">
         <f t="shared" si="0"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="S29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" t="s">
-        <v>97</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="S30" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>98</v>
@@ -2232,15 +2596,33 @@
       <c r="F31" t="s">
         <v>101</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="J31" t="s">
         <v>102</v>
       </c>
       <c r="M31" t="s">
         <v>98</v>
       </c>
+      <c r="N31" t="s">
+        <v>161</v>
+      </c>
+      <c r="O31" t="s">
+        <v>257</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q31">
+        <v>2.14</v>
+      </c>
       <c r="R31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.42</v>
+      </c>
+      <c r="S31" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2259,14 +2641,32 @@
       <c r="E32" t="s">
         <v>105</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N32" t="s">
+        <v>161</v>
+      </c>
+      <c r="O32" t="s">
+        <v>260</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q32">
+        <v>0.92</v>
+      </c>
       <c r="R32">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.92</v>
+      </c>
+      <c r="S32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
         <v>106</v>
@@ -2280,14 +2680,32 @@
       <c r="E33" t="s">
         <v>108</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N33" t="s">
+        <v>161</v>
+      </c>
+      <c r="O33" t="s">
+        <v>106</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q33">
+        <v>0.41</v>
+      </c>
       <c r="R33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.82</v>
+      </c>
+      <c r="S33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>109</v>
@@ -2301,12 +2719,27 @@
       <c r="E34" t="s">
         <v>111</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N34" t="s">
+        <v>161</v>
+      </c>
+      <c r="O34" t="s">
+        <v>266</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="R34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2322,14 +2755,26 @@
       <c r="E35" t="s">
         <v>113</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N35" t="s">
+        <v>161</v>
+      </c>
+      <c r="O35" t="s">
+        <v>266</v>
+      </c>
       <c r="R35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
         <v>114</v>
@@ -2346,12 +2791,27 @@
       <c r="F36" t="s">
         <v>117</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="N36" t="s">
+        <v>161</v>
+      </c>
+      <c r="O36" t="s">
+        <v>270</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>272</v>
+      </c>
       <c r="R36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2370,20 +2830,35 @@
       <c r="F37" t="s">
         <v>122</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="J37" t="s">
         <v>123</v>
       </c>
       <c r="L37" t="s">
         <v>124</v>
       </c>
+      <c r="N37" t="s">
+        <v>161</v>
+      </c>
+      <c r="O37" t="s">
+        <v>274</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="R37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>125</v>
@@ -2397,12 +2872,17 @@
       <c r="E38" t="s">
         <v>127</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="O38" s="5"/>
+      <c r="P38" s="4"/>
       <c r="R38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2418,12 +2898,27 @@
       <c r="E39" t="s">
         <v>130</v>
       </c>
+      <c r="N39" t="s">
+        <v>161</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q39">
+        <v>4.95</v>
+      </c>
       <c r="R39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>4.95</v>
+      </c>
+      <c r="S39" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2450,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2471,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2492,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2513,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2540,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2561,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -2582,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2615,8 +3110,21 @@
     <hyperlink ref="P15" r:id="rId5"/>
     <hyperlink ref="P17" r:id="rId6"/>
     <hyperlink ref="P19" r:id="rId7"/>
+    <hyperlink ref="P21" r:id="rId8"/>
+    <hyperlink ref="P23" r:id="rId9"/>
+    <hyperlink ref="P24" r:id="rId10"/>
+    <hyperlink ref="P27" r:id="rId11"/>
+    <hyperlink ref="P28" r:id="rId12"/>
+    <hyperlink ref="P29" r:id="rId13"/>
+    <hyperlink ref="P31" r:id="rId14"/>
+    <hyperlink ref="P32" r:id="rId15"/>
+    <hyperlink ref="P33" r:id="rId16"/>
+    <hyperlink ref="P34" r:id="rId17"/>
+    <hyperlink ref="P36" r:id="rId18"/>
+    <hyperlink ref="P37" r:id="rId19"/>
+    <hyperlink ref="P39" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed BOM spreadsheet, updated a part in a library.
</commit_message>
<xml_diff>
--- a/PCB/BOM_Spreadsheet.xlsx
+++ b/PCB/BOM_Spreadsheet.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="296">
   <si>
     <t>Qty</t>
   </si>
@@ -457,9 +457,6 @@
     <t>CR1</t>
   </si>
   <si>
-    <t>Bourns Electronics</t>
-  </si>
-  <si>
     <t>TPS2561DRCT</t>
   </si>
   <si>
@@ -493,9 +490,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
     <t>USB_TYPE_A</t>
   </si>
   <si>
@@ -847,9 +841,6 @@
     <t>AZ1117CR-3.3TRG1</t>
   </si>
   <si>
-    <t>not available</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/diodes-incorporated/AZ1117CR-3.3TRG1/AZ1117CR-3.3TRG1DICT-ND/5267011</t>
   </si>
   <si>
@@ -890,6 +881,66 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/sparkfun-electronics/COM-13910/1568-1391-ND/6023501</t>
+  </si>
+  <si>
+    <t>FDBL0260N100CT-ND</t>
+  </si>
+  <si>
+    <t>FDBL0260N100</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en/discrete-semiconductor-products/transistors-fets-mosfets-single/278?k=fdbl&amp;k=0260&amp;pkeyword=fdbl&amp;pv7=2&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>Already have some</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/fairchild-on-semiconductor/SMBJ13CA/SMBJ13CAFSCT-ND/3504357</t>
+  </si>
+  <si>
+    <t>SMBJ13CAFSCT-ND</t>
+  </si>
+  <si>
+    <t>not available / order from mouser</t>
+  </si>
+  <si>
+    <t>296-25548-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/TPS2561DRCT/296-25548-1-ND/2194871</t>
+  </si>
+  <si>
+    <t>296-46550-5-ND</t>
+  </si>
+  <si>
+    <t>TUSB4041IPAP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/TUSB4041IPAP/296-46550-5-ND/6572570</t>
+  </si>
+  <si>
+    <t>296-21527-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/TXB0108PWR/296-21527-1-ND/1305700</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/amphenol-commercial-products/UE27AC54100/UE27AC54100-ND/1972253</t>
+  </si>
+  <si>
+    <t>UE27AC54100-ND</t>
+  </si>
+  <si>
+    <t>UE27AC54100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ZXGD3009DYTADICT-ND</t>
+  </si>
+  <si>
+    <t>ZXGD3009DYTA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/diodes-incorporated/ZXGD3009DYTA/ZXGD3009DYTADICT-ND/5012618</t>
   </si>
 </sst>
 </file>
@@ -955,7 +1006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -969,6 +1020,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1291,8 +1345,8 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,19 +1413,19 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" t="s">
         <v>157</v>
       </c>
-      <c r="Q1" t="s">
-        <v>158</v>
-      </c>
-      <c r="R1" t="s">
-        <v>159</v>
-      </c>
       <c r="S1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1391,16 +1445,16 @@
         <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N2" t="s">
-        <v>161</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="P2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q2">
         <v>0.26</v>
@@ -1410,7 +1464,7 @@
         <v>0.78</v>
       </c>
       <c r="S2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1430,16 +1484,16 @@
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="N3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q3">
         <v>0.18</v>
@@ -1449,7 +1503,7 @@
         <v>1.7999999999999998</v>
       </c>
       <c r="S3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,16 +1523,16 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q4">
         <v>0.31</v>
@@ -1488,7 +1542,7 @@
         <v>1.55</v>
       </c>
       <c r="S4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1511,16 +1565,16 @@
         <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="Q5">
         <v>0.17</v>
@@ -1530,7 +1584,7 @@
         <v>6.8000000000000007</v>
       </c>
       <c r="S5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1553,16 +1607,16 @@
         <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="Q6">
         <v>0.1</v>
@@ -1572,7 +1626,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="S6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1595,16 +1649,16 @@
         <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P7" t="s">
         <v>182</v>
-      </c>
-      <c r="P7" t="s">
-        <v>184</v>
       </c>
       <c r="Q7">
         <v>1.0999999999999999E-2</v>
@@ -1614,7 +1668,7 @@
         <v>0.10999999999999999</v>
       </c>
       <c r="S7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1637,16 +1691,16 @@
         <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P8" t="s">
         <v>185</v>
-      </c>
-      <c r="P8" t="s">
-        <v>187</v>
       </c>
       <c r="Q8">
         <v>1.4E-2</v>
@@ -1656,7 +1710,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1664,7 +1718,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -1679,16 +1733,16 @@
         <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P9" t="s">
         <v>200</v>
-      </c>
-      <c r="P9" t="s">
-        <v>202</v>
       </c>
       <c r="Q9">
         <v>2.1000000000000001E-2</v>
@@ -1697,7 +1751,7 @@
         <v>0.19</v>
       </c>
       <c r="S9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1720,16 +1774,16 @@
         <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="P10" t="s">
         <v>188</v>
-      </c>
-      <c r="P10" t="s">
-        <v>190</v>
       </c>
       <c r="Q10">
         <v>2.7E-2</v>
@@ -1739,7 +1793,7 @@
         <v>0.27</v>
       </c>
       <c r="S10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1762,16 +1816,16 @@
         <v>37</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="P11" t="s">
         <v>192</v>
-      </c>
-      <c r="P11" t="s">
-        <v>194</v>
       </c>
       <c r="Q11">
         <v>0.13400000000000001</v>
@@ -1781,7 +1835,7 @@
         <v>2.0100000000000002</v>
       </c>
       <c r="S11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1804,16 +1858,16 @@
         <v>29</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="P12" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="Q12">
         <v>0.254</v>
@@ -1823,7 +1877,7 @@
         <v>2.54</v>
       </c>
       <c r="S12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1846,16 +1900,16 @@
         <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P13" t="s">
         <v>203</v>
-      </c>
-      <c r="P13" t="s">
-        <v>205</v>
       </c>
       <c r="Q13">
         <v>0.22</v>
@@ -1865,7 +1919,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="S13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1888,7 +1942,7 @@
         <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J14" t="s">
         <v>55</v>
@@ -1897,13 +1951,13 @@
         <v>50</v>
       </c>
       <c r="N14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O14" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="P14" t="s">
         <v>206</v>
-      </c>
-      <c r="P14" t="s">
-        <v>208</v>
       </c>
       <c r="Q14">
         <v>0.5</v>
@@ -1913,7 +1967,7 @@
         <v>1.5</v>
       </c>
       <c r="S14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1936,16 +1990,16 @@
         <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O15" t="s">
+        <v>207</v>
+      </c>
+      <c r="P15" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="Q15">
         <v>0.28000000000000003</v>
@@ -1955,7 +2009,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="S15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1978,16 +2032,16 @@
         <v>37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O16" t="s">
+        <v>210</v>
+      </c>
+      <c r="P16" t="s">
         <v>212</v>
-      </c>
-      <c r="P16" t="s">
-        <v>214</v>
       </c>
       <c r="Q16">
         <v>1.4E-2</v>
@@ -1997,7 +2051,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -2020,16 +2074,16 @@
         <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O17" t="s">
+        <v>213</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="Q17">
         <v>4.2999999999999997E-2</v>
@@ -2039,36 +2093,46 @@
         <v>0.42999999999999994</v>
       </c>
       <c r="S17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="6">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18">
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6">
         <v>2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="R18">
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="S18" s="6"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -2090,7 +2154,7 @@
         <v>69</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J19" t="s">
         <v>70</v>
@@ -2099,13 +2163,13 @@
         <v>71</v>
       </c>
       <c r="N19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O19" t="s">
+        <v>218</v>
+      </c>
+      <c r="P19" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="Q19">
         <v>7.4999999999999997E-2</v>
@@ -2115,7 +2179,7 @@
         <v>0.75</v>
       </c>
       <c r="S19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -2138,16 +2202,16 @@
         <v>29</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="N20" t="s">
+        <v>159</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="P20" t="s">
         <v>223</v>
-      </c>
-      <c r="N20" t="s">
-        <v>161</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="P20" t="s">
-        <v>225</v>
       </c>
       <c r="Q20">
         <v>0.49</v>
@@ -2157,7 +2221,7 @@
         <v>1.47</v>
       </c>
       <c r="S20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -2177,7 +2241,7 @@
         <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I21" t="s">
         <v>78</v>
@@ -2189,13 +2253,13 @@
         <v>74</v>
       </c>
       <c r="N21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q21">
         <v>0.73</v>
@@ -2205,7 +2269,7 @@
         <v>2.19</v>
       </c>
       <c r="S21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -2228,16 +2292,16 @@
         <v>37</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q22">
         <v>1.4E-2</v>
@@ -2247,7 +2311,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="S22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2270,16 +2334,16 @@
         <v>37</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="N23" t="s">
+        <v>159</v>
+      </c>
+      <c r="O23" t="s">
+        <v>233</v>
+      </c>
+      <c r="P23" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="N23" t="s">
-        <v>161</v>
-      </c>
-      <c r="O23" t="s">
-        <v>235</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="Q23">
         <v>1.0999999999999999E-2</v>
@@ -2289,7 +2353,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="S23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2312,16 +2376,16 @@
         <v>29</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Q24">
         <v>0.25</v>
@@ -2331,7 +2395,7 @@
         <v>1.25</v>
       </c>
       <c r="S24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -2354,16 +2418,16 @@
         <v>37</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O25" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="P25" t="s">
         <v>242</v>
-      </c>
-      <c r="P25" t="s">
-        <v>244</v>
       </c>
       <c r="Q25">
         <v>3.17</v>
@@ -2373,7 +2437,7 @@
         <v>6.34</v>
       </c>
       <c r="S25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2396,16 +2460,16 @@
         <v>37</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O26" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="P26" t="s">
         <v>245</v>
-      </c>
-      <c r="P26" t="s">
-        <v>247</v>
       </c>
       <c r="Q26">
         <v>1.2999999999999999E-2</v>
@@ -2415,7 +2479,7 @@
         <v>0.13</v>
       </c>
       <c r="S26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,16 +2499,16 @@
         <v>90</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q27">
         <v>0.59</v>
@@ -2454,7 +2518,7 @@
         <v>1.77</v>
       </c>
       <c r="S27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2477,16 +2541,16 @@
         <v>37</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Q28">
         <v>1.4E-2</v>
@@ -2496,7 +2560,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="S28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2519,16 +2583,16 @@
         <v>37</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Q29">
         <v>1.4E-2</v>
@@ -2538,7 +2602,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="S29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2574,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2597,7 +2661,7 @@
         <v>101</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J31" t="s">
         <v>102</v>
@@ -2606,13 +2670,13 @@
         <v>98</v>
       </c>
       <c r="N31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O31" t="s">
+        <v>255</v>
+      </c>
+      <c r="P31" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="P31" s="4" t="s">
-        <v>259</v>
       </c>
       <c r="Q31">
         <v>2.14</v>
@@ -2622,7 +2686,7 @@
         <v>6.42</v>
       </c>
       <c r="S31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2642,16 +2706,16 @@
         <v>105</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O32" t="s">
+        <v>258</v>
+      </c>
+      <c r="P32" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>262</v>
       </c>
       <c r="Q32">
         <v>0.92</v>
@@ -2661,7 +2725,7 @@
         <v>0.92</v>
       </c>
       <c r="S32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2681,16 +2745,16 @@
         <v>108</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O33" t="s">
         <v>106</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="Q33">
         <v>0.41</v>
@@ -2700,7 +2764,7 @@
         <v>0.82</v>
       </c>
       <c r="S33" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2720,56 +2784,68 @@
         <v>111</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O34" t="s">
+        <v>263</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q34">
+        <v>1.43</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="0"/>
+        <v>2.86</v>
+      </c>
+      <c r="S34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S35" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="P34" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S34" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>113</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="N35" t="s">
-        <v>161</v>
-      </c>
-      <c r="O35" t="s">
-        <v>266</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S35" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2792,23 +2868,26 @@
         <v>117</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="N36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O36" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
+      </c>
+      <c r="Q36">
+        <v>1.61</v>
       </c>
       <c r="R36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.22</v>
       </c>
       <c r="S36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2831,7 +2910,7 @@
         <v>122</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J37" t="s">
         <v>123</v>
@@ -2840,20 +2919,23 @@
         <v>124</v>
       </c>
       <c r="N37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O37" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
+      </c>
+      <c r="Q37">
+        <v>0.49</v>
       </c>
       <c r="R37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="S37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -2875,16 +2957,26 @@
       <c r="G38" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="4"/>
+      <c r="N38" t="s">
+        <v>159</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="R38">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="S38" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
         <v>128</v>
@@ -2898,29 +2990,32 @@
       <c r="E39" t="s">
         <v>130</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="N39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Q39">
         <v>4.95</v>
       </c>
       <c r="R39">
         <f t="shared" si="0"/>
-        <v>4.95</v>
+        <v>9.9</v>
       </c>
       <c r="S39" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>131</v>
@@ -2938,168 +3033,291 @@
         <v>131</v>
       </c>
       <c r="N40" t="s">
-        <v>134</v>
+        <v>159</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q40">
+        <v>0.37</v>
       </c>
       <c r="R40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="S40" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N41" t="s">
+        <v>159</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q41">
+        <v>2.87</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="0"/>
+        <v>8.61</v>
+      </c>
+      <c r="S41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
         <v>2</v>
       </c>
-      <c r="B41" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" t="s">
-        <v>135</v>
-      </c>
-      <c r="D41" t="s">
-        <v>136</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="B42" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="R41">
+      <c r="C42" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42" t="s">
-        <v>138</v>
-      </c>
-      <c r="C42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D42" t="s">
-        <v>138</v>
-      </c>
-      <c r="E42" t="s">
-        <v>139</v>
-      </c>
-      <c r="R42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="S42" s="6"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
         <v>140</v>
       </c>
-      <c r="C43" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>141</v>
       </c>
-      <c r="E43" t="s">
-        <v>142</v>
+      <c r="G43" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="N43" t="s">
+        <v>159</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q43">
+        <v>6.3</v>
       </c>
       <c r="R43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="S43" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" t="s">
         <v>143</v>
       </c>
-      <c r="C44" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>144</v>
       </c>
-      <c r="E44" t="s">
-        <v>145</v>
-      </c>
       <c r="G44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N44" t="s">
-        <v>146</v>
+        <v>159</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q44">
+        <v>1.59</v>
       </c>
       <c r="R44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.18</v>
+      </c>
+      <c r="S44" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="N45" t="s">
+        <v>159</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q45">
+        <v>0.378</v>
       </c>
       <c r="R45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="S45" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="N46" t="s">
+        <v>159</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q46">
+        <v>0.42</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="S46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
         <v>1</v>
       </c>
-      <c r="B46" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B47" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E46" t="s">
+      <c r="C47" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="R46">
+      <c r="D47" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" t="s">
-        <v>154</v>
-      </c>
-      <c r="E47" t="s">
-        <v>155</v>
-      </c>
-      <c r="F47" t="s">
-        <v>156</v>
-      </c>
-      <c r="R47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="S47" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3123,8 +3341,14 @@
     <hyperlink ref="P36" r:id="rId18"/>
     <hyperlink ref="P37" r:id="rId19"/>
     <hyperlink ref="P39" r:id="rId20"/>
+    <hyperlink ref="P40" r:id="rId21"/>
+    <hyperlink ref="P43" r:id="rId22"/>
+    <hyperlink ref="P41" r:id="rId23"/>
+    <hyperlink ref="P44" r:id="rId24"/>
+    <hyperlink ref="P45" r:id="rId25"/>
+    <hyperlink ref="P46" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>